<commit_message>
Scripts review, fix localization, add characters on scenes
</commit_message>
<xml_diff>
--- a/Assets/Spreadsheet/Scripts/Chapter3.xlsx
+++ b/Assets/Spreadsheet/Scripts/Chapter3.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Chapter3" sheetId="1" r:id="R1640a39de2e34e4c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Chapter3" sheetId="1" r:id="R72fd612d5b4741d0"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -16,6 +16,7 @@
     <x:t xml:space="preserve">@back Loc3.CircleReveal time:0.65
 @showUI MapButtonUI
 # Search
+@hideChars
 @hidePrinter 
 @choice  button:Items/Duck pos:-500,300 handler:ButtonArea goto:.Duck
 @choice  button:Items/WrongItem1 pos:700,125 handler:ButtonArea goto:.WrongItem
@@ -23,6 +24,7 @@
 @choice  button:Items/WrongItem3 pos:-50,250 handler:ButtonArea goto:.WrongItem
 @stop
 # Duck
+@char p look:right pos:50,7.5
 p: {0}
 </x:t>
   </x:si>
@@ -32,6 +34,8 @@
 @set "loc3_open = false"
 @stop
 # WrongItem
+@char p look:right pos:50,7.5
+@spawn ShakeCharacter params:p,2
 p: {0}
 </x:t>
   </x:si>

</xml_diff>